<commit_message>
commit for login page
</commit_message>
<xml_diff>
--- a/AutoationExersise/src/test/resources/ExcelData.xlsx
+++ b/AutoationExersise/src/test/resources/ExcelData.xlsx
@@ -72,7 +72,7 @@
     <t>Bhuli d Block</t>
   </si>
   <si>
-    <t>mitravinddar14bbbb@gmail.com</t>
+    <t>mitravindar14@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
commit for login changes
</commit_message>
<xml_diff>
--- a/AutoationExersise/src/test/resources/ExcelData.xlsx
+++ b/AutoationExersise/src/test/resources/ExcelData.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12516" windowHeight="2808"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12516" windowHeight="2808" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ContactUs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Ravindar</t>
   </si>
@@ -73,6 +74,12 @@
   </si>
   <si>
     <t>mitravindar14@gmail.com</t>
+  </si>
+  <si>
+    <t>Automation Testing</t>
+  </si>
+  <si>
+    <t>This site is very useful for beginer</t>
   </si>
 </sst>
 </file>
@@ -403,7 +410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -507,4 +514,41 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>